<commit_message>
Data in excel files condensed for ease of navigation
Unnecessary sheets were removed from the excel files. In this version, only the necessary data to reproduce the figures are kept. Please contact the authors for further inquiries.
</commit_message>
<xml_diff>
--- a/Figure 3.xlsx
+++ b/Figure 3.xlsx
@@ -5,16 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\PhD\1- Fossil Carbon Article\Nature Climate Change\New Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cdc895dc9b686e75/Belgeler/GitHub/FossilCarbon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8291604-881E-41F0-AC68-0D64CC825B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{E8291604-881E-41F0-AC68-0D64CC825B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF99A4AA-05C2-479D-BC91-83D2DEC10554}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="1092" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="1092" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Durable Accbysector&amp;prod 2011" sheetId="1" r:id="rId1"/>
-    <sheet name="Durable acc. 1995-2019" sheetId="2" r:id="rId2"/>
+    <sheet name="Figure 3" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,66 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
-  <si>
-    <t xml:space="preserve">Agriculture, Forestry and Fishing </t>
-  </si>
-  <si>
-    <t>Mining and Quarrying</t>
-  </si>
-  <si>
-    <t>Manufacturing</t>
-  </si>
-  <si>
-    <t>Electricity, Water and Gas for heating</t>
-  </si>
-  <si>
-    <t>Services</t>
-  </si>
-  <si>
-    <t>Recycling - Secondary raw materials for treatment</t>
-  </si>
-  <si>
-    <t>Waste treatment services</t>
-  </si>
-  <si>
-    <t>Final Demand</t>
-  </si>
-  <si>
-    <t>Textiles (17)</t>
-  </si>
-  <si>
-    <t>Leather and leather products (19)</t>
-  </si>
-  <si>
-    <t>Paper and paper products</t>
-  </si>
-  <si>
-    <t>Printed matter and recorded media (22)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Bitumen</t>
-  </si>
-  <si>
-    <t>Rubber and plastic products (25)</t>
-  </si>
-  <si>
-    <t>Glass and glass products</t>
-  </si>
-  <si>
-    <t>Iron, Steel, and metal structures</t>
-  </si>
-  <si>
-    <t>Heterogeneous Machinery</t>
-  </si>
-  <si>
-    <t>Motor vehicles; trailers and semi-trailers (34)</t>
-  </si>
-  <si>
-    <t>Mix (%)</t>
-  </si>
-  <si>
-    <t>Total (Mt)</t>
   </si>
   <si>
     <t>CO2 Emissions (FC. Eq.)</t>
@@ -163,16 +105,8 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -193,24 +127,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -255,7 +177,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -263,106 +185,19 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -417,7 +252,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Durable acc. 1995-2019'!$A$2</c:f>
+              <c:f>'Figure 3'!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -438,7 +273,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$1:$Z$1</c:f>
+              <c:f>'Figure 3'!$B$1:$Z$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -522,7 +357,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$2:$Z$2</c:f>
+              <c:f>'Figure 3'!$B$2:$Z$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -615,7 +450,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Durable acc. 1995-2019'!$A$3</c:f>
+              <c:f>'Figure 3'!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -636,7 +471,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$1:$Z$1</c:f>
+              <c:f>'Figure 3'!$B$1:$Z$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -720,7 +555,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$3:$Z$3</c:f>
+              <c:f>'Figure 3'!$B$3:$Z$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -813,7 +648,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Durable acc. 1995-2019'!$A$4</c:f>
+              <c:f>'Figure 3'!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -834,7 +669,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$1:$Z$1</c:f>
+              <c:f>'Figure 3'!$B$1:$Z$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -918,7 +753,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$4:$Z$4</c:f>
+              <c:f>'Figure 3'!$B$4:$Z$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1011,7 +846,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Durable acc. 1995-2019'!$A$5</c:f>
+              <c:f>'Figure 3'!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1032,7 +867,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$1:$Z$1</c:f>
+              <c:f>'Figure 3'!$B$1:$Z$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1116,7 +951,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$5:$Z$5</c:f>
+              <c:f>'Figure 3'!$B$5:$Z$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1209,7 +1044,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Durable acc. 1995-2019'!$A$6</c:f>
+              <c:f>'Figure 3'!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1230,7 +1065,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$1:$Z$1</c:f>
+              <c:f>'Figure 3'!$B$1:$Z$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1314,7 +1149,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$6:$Z$6</c:f>
+              <c:f>'Figure 3'!$B$6:$Z$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1407,7 +1242,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Durable acc. 1995-2019'!$A$7</c:f>
+              <c:f>'Figure 3'!$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1428,7 +1263,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$1:$Z$1</c:f>
+              <c:f>'Figure 3'!$B$1:$Z$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1512,7 +1347,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$7:$Z$7</c:f>
+              <c:f>'Figure 3'!$B$7:$Z$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1605,7 +1440,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Durable acc. 1995-2019'!$A$8</c:f>
+              <c:f>'Figure 3'!$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1628,7 +1463,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$1:$Z$1</c:f>
+              <c:f>'Figure 3'!$B$1:$Z$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1712,7 +1547,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$8:$Z$8</c:f>
+              <c:f>'Figure 3'!$B$8:$Z$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1805,7 +1640,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Durable acc. 1995-2019'!$A$9</c:f>
+              <c:f>'Figure 3'!$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1828,7 +1663,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$1:$Z$1</c:f>
+              <c:f>'Figure 3'!$B$1:$Z$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1912,7 +1747,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$9:$Z$9</c:f>
+              <c:f>'Figure 3'!$B$9:$Z$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -2005,7 +1840,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Durable acc. 1995-2019'!$A$10</c:f>
+              <c:f>'Figure 3'!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2028,7 +1863,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$1:$Z$1</c:f>
+              <c:f>'Figure 3'!$B$1:$Z$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -2112,7 +1947,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$10:$Z$10</c:f>
+              <c:f>'Figure 3'!$B$10:$Z$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -2205,7 +2040,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Durable acc. 1995-2019'!$A$11</c:f>
+              <c:f>'Figure 3'!$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2228,7 +2063,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$1:$Z$1</c:f>
+              <c:f>'Figure 3'!$B$1:$Z$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -2312,7 +2147,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$11:$Z$11</c:f>
+              <c:f>'Figure 3'!$B$11:$Z$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -2405,7 +2240,7 @@
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Durable acc. 1995-2019'!$A$12</c:f>
+              <c:f>'Figure 3'!$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2428,7 +2263,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$1:$Z$1</c:f>
+              <c:f>'Figure 3'!$B$1:$Z$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -2512,7 +2347,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$12:$Z$12</c:f>
+              <c:f>'Figure 3'!$B$12:$Z$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -2605,7 +2440,7 @@
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Durable acc. 1995-2019'!$A$13</c:f>
+              <c:f>'Figure 3'!$A$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2628,7 +2463,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$1:$Z$1</c:f>
+              <c:f>'Figure 3'!$B$1:$Z$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -2712,7 +2547,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$13:$Z$13</c:f>
+              <c:f>'Figure 3'!$B$13:$Z$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -2805,7 +2640,7 @@
           <c:order val="12"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Durable acc. 1995-2019'!$A$14</c:f>
+              <c:f>'Figure 3'!$A$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2829,7 +2664,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$1:$Z$1</c:f>
+              <c:f>'Figure 3'!$B$1:$Z$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -2913,7 +2748,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$14:$Z$14</c:f>
+              <c:f>'Figure 3'!$B$14:$Z$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -3006,7 +2841,7 @@
           <c:order val="13"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Durable acc. 1995-2019'!$A$15</c:f>
+              <c:f>'Figure 3'!$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3030,7 +2865,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$1:$Z$1</c:f>
+              <c:f>'Figure 3'!$B$1:$Z$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -3114,7 +2949,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$15:$Z$15</c:f>
+              <c:f>'Figure 3'!$B$15:$Z$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -3207,7 +3042,7 @@
           <c:order val="14"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Durable acc. 1995-2019'!$A$16</c:f>
+              <c:f>'Figure 3'!$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3231,7 +3066,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$1:$Z$1</c:f>
+              <c:f>'Figure 3'!$B$1:$Z$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -3315,7 +3150,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$16:$Z$16</c:f>
+              <c:f>'Figure 3'!$B$16:$Z$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -3408,7 +3243,7 @@
           <c:order val="15"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Durable acc. 1995-2019'!$A$17</c:f>
+              <c:f>'Figure 3'!$A$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3432,7 +3267,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$1:$Z$1</c:f>
+              <c:f>'Figure 3'!$B$1:$Z$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -3516,7 +3351,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$17:$Z$17</c:f>
+              <c:f>'Figure 3'!$B$17:$Z$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -3625,7 +3460,7 @@
           <c:order val="16"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Durable acc. 1995-2019'!$A$18</c:f>
+              <c:f>'Figure 3'!$A$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3669,7 +3504,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$1:$Z$1</c:f>
+              <c:f>'Figure 3'!$B$1:$Z$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -3753,7 +3588,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$18:$Z$18</c:f>
+              <c:f>'Figure 3'!$B$18:$Z$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -3847,7 +3682,7 @@
           <c:order val="17"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Durable acc. 1995-2019'!$A$19</c:f>
+              <c:f>'Figure 3'!$A$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4211,7 +4046,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$1:$Z$1</c:f>
+              <c:f>'Figure 3'!$B$1:$Z$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -4295,7 +4130,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Durable acc. 1995-2019'!$B$19:$Z$19</c:f>
+              <c:f>'Figure 3'!$B$19:$Z$19</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="25"/>
@@ -5431,6 +5266,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5693,518 +5532,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2">
-        <v>4.7481078010987804E-2</v>
-      </c>
-      <c r="C2">
-        <v>5.1954412249662404E-3</v>
-      </c>
-      <c r="D2">
-        <v>1.7956588100573414</v>
-      </c>
-      <c r="E2">
-        <v>4.7784502881495997E-3</v>
-      </c>
-      <c r="F2">
-        <v>1.4003160791902318</v>
-      </c>
-      <c r="G2">
-        <v>8.9327232276832007E-4</v>
-      </c>
-      <c r="H2">
-        <v>6.9147819070559998E-3</v>
-      </c>
-      <c r="I2">
-        <v>0.13123798028467099</v>
-      </c>
-      <c r="J2">
-        <f>SUM(B2:I2)</f>
-        <v>3.3924758932861718</v>
-      </c>
-      <c r="K2">
-        <f>J2/$J$12*100</f>
-        <v>0.95484625181727378</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>1.0544976335946501E-2</v>
-      </c>
-      <c r="C3">
-        <v>6.9116019763144822E-3</v>
-      </c>
-      <c r="D3">
-        <v>0.20782113665656793</v>
-      </c>
-      <c r="E3">
-        <v>9.7777021741260409E-3</v>
-      </c>
-      <c r="F3">
-        <v>5.0261442038345656E-2</v>
-      </c>
-      <c r="G3">
-        <v>7.0083646945273497E-4</v>
-      </c>
-      <c r="H3">
-        <v>4.0894128661907603E-3</v>
-      </c>
-      <c r="I3">
-        <v>5.275991780712509E-4</v>
-      </c>
-      <c r="J3">
-        <f t="shared" ref="J3:J11" si="0">SUM(B3:I3)</f>
-        <v>0.29063470769501537</v>
-      </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K11" si="1">J3/$J$12*100</f>
-        <v>8.1802043704952865E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4">
-        <v>8.6301166696323914E-3</v>
-      </c>
-      <c r="C4">
-        <v>3.2986373489247403E-3</v>
-      </c>
-      <c r="D4">
-        <v>1.0897792354924463</v>
-      </c>
-      <c r="E4">
-        <v>4.2850614034489103E-3</v>
-      </c>
-      <c r="F4">
-        <v>0.62001838829243683</v>
-      </c>
-      <c r="G4">
-        <v>4.6942022392738704E-3</v>
-      </c>
-      <c r="H4">
-        <v>7.0348276005996798E-3</v>
-      </c>
-      <c r="I4">
-        <v>6.9238401079285902E-3</v>
-      </c>
-      <c r="J4">
-        <f t="shared" si="0"/>
-        <v>1.7446643091546912</v>
-      </c>
-      <c r="K4">
-        <f t="shared" si="1"/>
-        <v>0.49105320971405497</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5">
-        <v>2.8499683092667598E-3</v>
-      </c>
-      <c r="C5">
-        <v>4.8993677259120084E-3</v>
-      </c>
-      <c r="D5">
-        <v>0.76233138000663259</v>
-      </c>
-      <c r="E5">
-        <v>1.3856622799165165E-2</v>
-      </c>
-      <c r="F5">
-        <v>1.6967992340564169</v>
-      </c>
-      <c r="G5">
-        <v>2.3381041020054901E-3</v>
-      </c>
-      <c r="H5">
-        <v>5.9404502182216403E-3</v>
-      </c>
-      <c r="I5">
-        <v>4.3518796854031004E-2</v>
-      </c>
-      <c r="J5">
-        <f t="shared" si="0"/>
-        <v>2.5325339240716516</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="1"/>
-        <v>0.71280698848459689</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>93.381379755339594</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>5.4057263304820606E-3</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="0"/>
-        <v>93.386785481670074</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="1"/>
-        <v>26.284644280864917</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7">
-        <v>1.25739250956335</v>
-      </c>
-      <c r="C7">
-        <v>0.9433791824177773</v>
-      </c>
-      <c r="D7">
-        <v>46.618662180284986</v>
-      </c>
-      <c r="E7">
-        <v>0.24180400831611043</v>
-      </c>
-      <c r="F7">
-        <v>32.452036262022411</v>
-      </c>
-      <c r="G7">
-        <v>0.54037741101063097</v>
-      </c>
-      <c r="H7">
-        <v>0.18453051859551198</v>
-      </c>
-      <c r="I7">
-        <v>1.1753647914248402</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="0"/>
-        <v>83.413546863635602</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="1"/>
-        <v>23.477576577965191</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8">
-        <v>6.9491325480216699E-3</v>
-      </c>
-      <c r="C8">
-        <v>5.7092841003684768E-3</v>
-      </c>
-      <c r="D8">
-        <v>0.15104812072462556</v>
-      </c>
-      <c r="E8">
-        <v>1.2596117743909111E-3</v>
-      </c>
-      <c r="F8">
-        <v>0.19070792291957203</v>
-      </c>
-      <c r="G8">
-        <v>1.83727385697923E-2</v>
-      </c>
-      <c r="H8">
-        <v>5.8968391539186899E-4</v>
-      </c>
-      <c r="I8">
-        <v>1.95595476942589E-3</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="0"/>
-        <v>0.37659244932158875</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="1"/>
-        <v>0.10599570933106485</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9">
-        <v>8.8011753971382001E-2</v>
-      </c>
-      <c r="C9">
-        <v>0.17172254256514025</v>
-      </c>
-      <c r="D9">
-        <v>9.1951522553099689</v>
-      </c>
-      <c r="E9">
-        <v>9.0333855120169795E-2</v>
-      </c>
-      <c r="F9">
-        <v>6.8781749530355363</v>
-      </c>
-      <c r="G9">
-        <v>0.128020963794168</v>
-      </c>
-      <c r="H9">
-        <v>1.9365732747178999E-2</v>
-      </c>
-      <c r="I9">
-        <v>1.7790708540882456</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="0"/>
-        <v>18.349852910631789</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="1"/>
-        <v>5.1647495293305683</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10">
-        <v>0.54459391712331007</v>
-      </c>
-      <c r="C10">
-        <v>1.7311384000690022</v>
-      </c>
-      <c r="D10">
-        <v>22.360892874252425</v>
-      </c>
-      <c r="E10">
-        <v>1.7668624627805962</v>
-      </c>
-      <c r="F10">
-        <v>25.059046765099037</v>
-      </c>
-      <c r="G10">
-        <v>0.52998844705358694</v>
-      </c>
-      <c r="H10">
-        <v>0.47627932468583317</v>
-      </c>
-      <c r="I10">
-        <v>77.139291484360342</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="0"/>
-        <v>129.60809367542413</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="1"/>
-        <v>36.479493545135547</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11">
-        <v>0.15334039829340501</v>
-      </c>
-      <c r="C11">
-        <v>6.4620689755192404E-2</v>
-      </c>
-      <c r="D11">
-        <v>8.8911233165784456</v>
-      </c>
-      <c r="E11">
-        <v>4.0424838700954972E-2</v>
-      </c>
-      <c r="F11">
-        <v>2.2308396094823451</v>
-      </c>
-      <c r="G11">
-        <v>1.37256099319732E-2</v>
-      </c>
-      <c r="H11">
-        <v>6.7022351739506492E-2</v>
-      </c>
-      <c r="I11">
-        <v>10.734</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="0"/>
-        <v>22.195096814481822</v>
-      </c>
-      <c r="K11">
-        <f t="shared" si="1"/>
-        <v>6.2470318636518485</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12">
-        <f>SUM(B2:B11)</f>
-        <v>2.1197938508253023</v>
-      </c>
-      <c r="C12">
-        <f t="shared" ref="C12:I12" si="2">SUM(C2:C11)</f>
-        <v>2.9368751471835979</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="2"/>
-        <v>91.072469309363441</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="2"/>
-        <v>2.1733826133571124</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="2"/>
-        <v>163.95958041147594</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="2"/>
-        <v>1.2391115854936516</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="2"/>
-        <v>0.77176708427549068</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="2"/>
-        <v>91.01729702739803</v>
-      </c>
-      <c r="J12">
-        <f>SUM(J2:J11)</f>
-        <v>355.29027702937248</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13">
-        <f>B12/$J$12*100</f>
-        <v>0.59663716906332764</v>
-      </c>
-      <c r="C13">
-        <f t="shared" ref="C13:I13" si="3">C12/$J$12*100</f>
-        <v>0.8266128675794866</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="3"/>
-        <v>25.633256859949004</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="3"/>
-        <v>0.61172026195848728</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="3"/>
-        <v>46.148062869145477</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="3"/>
-        <v>0.3487603420656547</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="3"/>
-        <v>0.21722156055840711</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="3"/>
-        <v>25.617728069680179</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E21F4772-9AF2-4876-B999-091AF688E769}">
   <dimension ref="A1:BA19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB42" sqref="AB42"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:53" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="B1">
         <v>1995</v>
@@ -6282,12 +5621,12 @@
         <v>2019</v>
       </c>
       <c r="AC1" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
-        <v>22</v>
+      <c r="A2" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B2">
         <f>AC2/12*44</f>
@@ -6466,8 +5805,8 @@
       </c>
     </row>
     <row r="3" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
-        <v>23</v>
+      <c r="A3" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B17" si="1">AC3/12*44</f>
@@ -6646,8 +5985,8 @@
       </c>
     </row>
     <row r="4" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
-        <v>24</v>
+      <c r="A4" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B4">
         <f t="shared" si="1"/>
@@ -6826,8 +6165,8 @@
       </c>
     </row>
     <row r="5" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
-        <v>25</v>
+      <c r="A5" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B5">
         <f t="shared" si="1"/>
@@ -7006,8 +6345,8 @@
       </c>
     </row>
     <row r="6" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
-        <v>12</v>
+      <c r="A6" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="B6">
         <f t="shared" si="1"/>
@@ -7186,8 +6525,8 @@
       </c>
     </row>
     <row r="7" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
-        <v>26</v>
+      <c r="A7" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="B7">
         <f t="shared" si="1"/>
@@ -7366,8 +6705,8 @@
       </c>
     </row>
     <row r="8" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
-        <v>27</v>
+      <c r="A8" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="B8">
         <f t="shared" si="1"/>
@@ -7546,8 +6885,8 @@
       </c>
     </row>
     <row r="9" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
-        <v>28</v>
+      <c r="A9" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="B9">
         <f t="shared" si="1"/>
@@ -7726,8 +7065,8 @@
       </c>
     </row>
     <row r="10" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
-        <v>29</v>
+      <c r="A10" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="B10">
         <f t="shared" si="1"/>
@@ -7906,8 +7245,8 @@
       </c>
     </row>
     <row r="11" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
-        <v>30</v>
+      <c r="A11" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="B11">
         <f t="shared" si="1"/>
@@ -8086,8 +7425,8 @@
       </c>
     </row>
     <row r="12" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
-        <v>31</v>
+      <c r="A12" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="B12">
         <f t="shared" si="1"/>
@@ -8266,8 +7605,8 @@
       </c>
     </row>
     <row r="13" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A13" s="16" t="s">
-        <v>32</v>
+      <c r="A13" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="B13">
         <f t="shared" si="1"/>
@@ -8446,8 +7785,8 @@
       </c>
     </row>
     <row r="14" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
-        <v>33</v>
+      <c r="A14" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="B14">
         <f t="shared" si="1"/>
@@ -8626,8 +7965,8 @@
       </c>
     </row>
     <row r="15" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A15" s="16" t="s">
-        <v>34</v>
+      <c r="A15" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="B15">
         <f t="shared" si="1"/>
@@ -8806,8 +8145,8 @@
       </c>
     </row>
     <row r="16" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
-        <v>35</v>
+      <c r="A16" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="B16">
         <f t="shared" si="1"/>
@@ -8986,8 +8325,8 @@
       </c>
     </row>
     <row r="17" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A17" s="16" t="s">
-        <v>36</v>
+      <c r="A17" s="6" t="s">
+        <v>17</v>
       </c>
       <c r="B17">
         <f t="shared" si="1"/>
@@ -9166,8 +8505,8 @@
       </c>
     </row>
     <row r="18" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A18" s="16" t="s">
-        <v>20</v>
+      <c r="A18" s="6" t="s">
+        <v>1</v>
       </c>
       <c r="B18">
         <v>23.458714000000001</v>
@@ -9321,106 +8660,106 @@
       </c>
     </row>
     <row r="19" spans="1:53" x14ac:dyDescent="0.3">
-      <c r="A19" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="18">
+      <c r="A19" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="8">
         <f>SUM(B2:B17)/B18</f>
         <v>2.1368076603138518E-2</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="8">
         <f t="shared" ref="C19:Z19" si="26">SUM(C2:C17)/C18</f>
         <v>2.135811440798625E-2</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="8">
         <f t="shared" si="26"/>
         <v>2.2831308465133711E-2</v>
       </c>
-      <c r="E19" s="18">
+      <c r="E19" s="8">
         <f t="shared" si="26"/>
         <v>2.5053685166964934E-2</v>
       </c>
-      <c r="F19" s="18">
+      <c r="F19" s="8">
         <f t="shared" si="26"/>
         <v>2.5241433780201321E-2</v>
       </c>
-      <c r="G19" s="18">
+      <c r="G19" s="8">
         <f t="shared" si="26"/>
         <v>2.6859577155465435E-2</v>
       </c>
-      <c r="H19" s="18">
+      <c r="H19" s="8">
         <f t="shared" si="26"/>
         <v>2.6866148786906737E-2</v>
       </c>
-      <c r="I19" s="18">
+      <c r="I19" s="8">
         <f t="shared" si="26"/>
         <v>2.78960790812476E-2</v>
       </c>
-      <c r="J19" s="18">
+      <c r="J19" s="8">
         <f t="shared" si="26"/>
         <v>2.6691170129771308E-2</v>
       </c>
-      <c r="K19" s="18">
+      <c r="K19" s="8">
         <f t="shared" si="26"/>
         <v>2.9301510831935936E-2</v>
       </c>
-      <c r="L19" s="18">
+      <c r="L19" s="8">
         <f t="shared" si="26"/>
         <v>3.1406337677277678E-2</v>
       </c>
-      <c r="M19" s="18">
+      <c r="M19" s="8">
         <f t="shared" si="26"/>
         <v>3.4075292044804549E-2</v>
       </c>
-      <c r="N19" s="18">
+      <c r="N19" s="8">
         <f t="shared" si="26"/>
         <v>3.5947982405873664E-2</v>
       </c>
-      <c r="O19" s="18">
+      <c r="O19" s="8">
         <f t="shared" si="26"/>
         <v>3.5983543929276246E-2</v>
       </c>
-      <c r="P19" s="18">
+      <c r="P19" s="8">
         <f t="shared" si="26"/>
         <v>3.1640199062623206E-2</v>
       </c>
-      <c r="Q19" s="18">
+      <c r="Q19" s="8">
         <f t="shared" si="26"/>
         <v>3.7831116248864614E-2</v>
       </c>
-      <c r="R19" s="18">
+      <c r="R19" s="8">
         <f t="shared" si="26"/>
         <v>3.7769620437792126E-2</v>
       </c>
-      <c r="S19" s="18">
+      <c r="S19" s="8">
         <f t="shared" si="26"/>
         <v>3.9144881636607953E-2</v>
       </c>
-      <c r="T19" s="18">
+      <c r="T19" s="8">
         <f t="shared" si="26"/>
         <v>4.078333677594316E-2</v>
       </c>
-      <c r="U19" s="18">
+      <c r="U19" s="8">
         <f t="shared" si="26"/>
         <v>4.0779016588736297E-2</v>
       </c>
-      <c r="V19" s="18">
+      <c r="V19" s="8">
         <f t="shared" si="26"/>
         <v>4.8158696634980493E-2</v>
       </c>
-      <c r="W19" s="18">
+      <c r="W19" s="8">
         <f t="shared" si="26"/>
         <v>4.8374347487769698E-2</v>
       </c>
-      <c r="X19" s="18">
+      <c r="X19" s="8">
         <f t="shared" si="26"/>
         <v>5.2034223638868476E-2</v>
       </c>
-      <c r="Y19" s="18">
+      <c r="Y19" s="8">
         <f t="shared" si="26"/>
         <v>5.9624184525545097E-2</v>
       </c>
-      <c r="Z19" s="18">
+      <c r="Z19" s="8">
         <f t="shared" si="26"/>
         <v>6.5416558487515014E-2</v>
       </c>

</xml_diff>